<commit_message>
feat: newest stable version
</commit_message>
<xml_diff>
--- a/bubble-video/formatted_data.xlsx
+++ b/bubble-video/formatted_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/130fda80f0432a83/Files/000_Archive/TravelMarketViz/bubble-video/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_FFC65FC0D0E169F172170B557353052D6C88EFDE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC90DA52-6267-134B-88AB-14D9E127CEDE}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_FFC65FC0D0E169F172170B557353052D6C88EFDE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F47E743-9085-174B-9824-E379FACE2F55}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -829,11 +829,15 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F1382"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I808" sqref="I808"/>
+    <sheetView tabSelected="1" topLeftCell="A336" zoomScale="228" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
+    <col min="6" max="6" width="33.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -855,7 +859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -869,7 +873,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -883,7 +887,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -897,7 +901,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -914,7 +918,7 @@
         <v>-13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -931,7 +935,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -948,7 +952,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -965,7 +969,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -985,7 +989,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1005,7 +1009,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1025,7 +1029,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1045,7 +1049,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1065,7 +1069,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1085,7 +1089,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1105,7 +1109,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1125,7 +1129,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1145,7 +1149,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1165,7 +1169,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1185,7 +1189,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1205,7 +1209,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1225,7 +1229,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1245,7 +1249,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1265,7 +1269,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1285,7 +1289,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1305,7 +1309,7 @@
         <v>-28</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1325,7 +1329,7 @@
         <v>-27</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1345,7 +1349,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1365,7 +1369,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1385,7 +1389,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1405,7 +1409,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1425,7 +1429,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1445,7 +1449,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1465,7 +1469,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1485,7 +1489,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1505,7 +1509,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1525,7 +1529,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1545,7 +1549,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1565,7 +1569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1585,7 +1589,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1605,7 +1609,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -2051,7 +2055,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -2065,7 +2069,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -2079,7 +2083,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -2093,7 +2097,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -2110,7 +2114,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -2127,7 +2131,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -2144,7 +2148,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -2161,7 +2165,7 @@
         <v>-47</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -2178,7 +2182,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -2198,7 +2202,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -2218,7 +2222,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -2238,7 +2242,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -2258,7 +2262,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -2278,7 +2282,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -2298,7 +2302,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>8</v>
       </c>
@@ -2318,7 +2322,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -2338,7 +2342,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>8</v>
       </c>
@@ -2358,7 +2362,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -2378,7 +2382,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -2398,7 +2402,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -2418,7 +2422,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -2438,7 +2442,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -2458,7 +2462,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>8</v>
       </c>
@@ -2478,7 +2482,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -2498,7 +2502,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>8</v>
       </c>
@@ -2518,7 +2522,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>8</v>
       </c>
@@ -2538,7 +2542,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -2558,7 +2562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -2578,7 +2582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>8</v>
       </c>
@@ -2598,7 +2602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>8</v>
       </c>
@@ -2618,7 +2622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -2638,7 +2642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>8</v>
       </c>
@@ -2658,7 +2662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>8</v>
       </c>
@@ -2678,7 +2682,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>8</v>
       </c>
@@ -2698,7 +2702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>8</v>
       </c>
@@ -2718,7 +2722,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>8</v>
       </c>
@@ -2738,7 +2742,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>8</v>
       </c>
@@ -2758,7 +2762,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>8</v>
       </c>
@@ -2778,7 +2782,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>8</v>
       </c>
@@ -2798,7 +2802,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>8</v>
       </c>
@@ -2818,7 +2822,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>8</v>
       </c>
@@ -2838,7 +2842,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>8</v>
       </c>
@@ -2858,7 +2862,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>8</v>
       </c>
@@ -2878,7 +2882,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>8</v>
       </c>
@@ -2898,7 +2902,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>8</v>
       </c>
@@ -2918,7 +2922,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>8</v>
       </c>
@@ -2938,7 +2942,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>8</v>
       </c>
@@ -2958,7 +2962,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>8</v>
       </c>
@@ -2978,7 +2982,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>8</v>
       </c>
@@ -2998,7 +3002,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>8</v>
       </c>
@@ -3018,7 +3022,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>8</v>
       </c>
@@ -3038,7 +3042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>8</v>
       </c>
@@ -3058,7 +3062,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>8</v>
       </c>
@@ -3078,7 +3082,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>8</v>
       </c>
@@ -3098,7 +3102,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>8</v>
       </c>
@@ -3118,7 +3122,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>8</v>
       </c>
@@ -3138,7 +3142,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>8</v>
       </c>
@@ -3158,7 +3162,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>8</v>
       </c>
@@ -3178,7 +3182,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>8</v>
       </c>
@@ -3198,7 +3202,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>8</v>
       </c>
@@ -3218,7 +3222,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>8</v>
       </c>
@@ -3238,7 +3242,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>8</v>
       </c>
@@ -3258,7 +3262,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>8</v>
       </c>
@@ -3278,7 +3282,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>8</v>
       </c>
@@ -3298,7 +3302,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>8</v>
       </c>
@@ -3318,7 +3322,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>8</v>
       </c>
@@ -3338,7 +3342,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>8</v>
       </c>
@@ -3358,7 +3362,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>8</v>
       </c>
@@ -3378,7 +3382,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>8</v>
       </c>
@@ -3398,7 +3402,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>8</v>
       </c>
@@ -3418,7 +3422,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>8</v>
       </c>
@@ -3438,7 +3442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>8</v>
       </c>
@@ -3458,7 +3462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>8</v>
       </c>
@@ -3478,7 +3482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>8</v>
       </c>
@@ -3498,7 +3502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>8</v>
       </c>
@@ -3518,7 +3522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>8</v>
       </c>
@@ -3538,7 +3542,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>8</v>
       </c>
@@ -3558,7 +3562,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>8</v>
       </c>
@@ -3578,7 +3582,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>8</v>
       </c>
@@ -3598,7 +3602,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>8</v>
       </c>
@@ -3618,7 +3622,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>8</v>
       </c>
@@ -3638,7 +3642,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>8</v>
       </c>
@@ -3658,7 +3662,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>8</v>
       </c>
@@ -3678,7 +3682,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>8</v>
       </c>
@@ -3698,7 +3702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>8</v>
       </c>
@@ -3718,7 +3722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>8</v>
       </c>
@@ -3738,7 +3742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>8</v>
       </c>
@@ -3758,7 +3762,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>8</v>
       </c>
@@ -3778,7 +3782,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>8</v>
       </c>
@@ -3798,7 +3802,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>8</v>
       </c>
@@ -3818,7 +3822,7 @@
         <v>-24</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>8</v>
       </c>
@@ -3838,7 +3842,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>8</v>
       </c>
@@ -3858,7 +3862,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>8</v>
       </c>
@@ -3878,7 +3882,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>8</v>
       </c>
@@ -3898,7 +3902,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>8</v>
       </c>
@@ -3918,7 +3922,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>8</v>
       </c>
@@ -3938,7 +3942,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>8</v>
       </c>
@@ -3958,7 +3962,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>8</v>
       </c>
@@ -3978,7 +3982,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>8</v>
       </c>
@@ -3998,7 +4002,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>8</v>
       </c>
@@ -4018,7 +4022,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>8</v>
       </c>
@@ -4038,7 +4042,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>8</v>
       </c>
@@ -4058,7 +4062,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>8</v>
       </c>
@@ -4078,7 +4082,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>8</v>
       </c>
@@ -4098,7 +4102,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>8</v>
       </c>
@@ -4118,7 +4122,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>8</v>
       </c>
@@ -4138,7 +4142,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>8</v>
       </c>
@@ -4158,7 +4162,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>8</v>
       </c>
@@ -6545,7 +6549,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="297" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>12</v>
       </c>
@@ -6559,7 +6563,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>12</v>
       </c>
@@ -6573,7 +6577,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="299" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>12</v>
       </c>
@@ -6587,7 +6591,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="300" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>12</v>
       </c>
@@ -6601,7 +6605,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="301" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>12</v>
       </c>
@@ -6618,7 +6622,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="302" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>12</v>
       </c>
@@ -6635,7 +6639,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="303" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>12</v>
       </c>
@@ -6652,7 +6656,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="304" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>12</v>
       </c>
@@ -6669,7 +6673,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="305" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>12</v>
       </c>
@@ -6686,7 +6690,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>12</v>
       </c>
@@ -6703,7 +6707,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="307" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>12</v>
       </c>
@@ -6720,7 +6724,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="308" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>12</v>
       </c>
@@ -6740,7 +6744,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="309" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>12</v>
       </c>
@@ -6760,7 +6764,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="310" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>12</v>
       </c>
@@ -6780,7 +6784,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="311" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>12</v>
       </c>
@@ -6800,7 +6804,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="312" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>12</v>
       </c>
@@ -6820,7 +6824,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="313" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>12</v>
       </c>
@@ -6840,7 +6844,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="314" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>12</v>
       </c>
@@ -6860,7 +6864,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="315" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>12</v>
       </c>
@@ -6880,7 +6884,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="316" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>12</v>
       </c>
@@ -6900,7 +6904,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="317" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>12</v>
       </c>
@@ -6920,7 +6924,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="318" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>12</v>
       </c>
@@ -6940,7 +6944,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="319" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>12</v>
       </c>
@@ -6960,7 +6964,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="320" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>12</v>
       </c>
@@ -6980,7 +6984,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="321" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>12</v>
       </c>
@@ -7000,7 +7004,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="322" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>12</v>
       </c>
@@ -7020,7 +7024,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="323" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>12</v>
       </c>
@@ -7040,7 +7044,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="324" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>12</v>
       </c>
@@ -7060,7 +7064,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="325" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>12</v>
       </c>
@@ -7080,7 +7084,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="326" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>12</v>
       </c>
@@ -7100,7 +7104,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="327" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>12</v>
       </c>
@@ -7120,7 +7124,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="328" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>12</v>
       </c>
@@ -7140,7 +7144,7 @@
         <v>-21</v>
       </c>
     </row>
-    <row r="329" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>12</v>
       </c>
@@ -7160,7 +7164,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="330" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>12</v>
       </c>
@@ -7180,7 +7184,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="331" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>12</v>
       </c>
@@ -7200,7 +7204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="332" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>12</v>
       </c>
@@ -7220,7 +7224,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="333" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>12</v>
       </c>
@@ -7240,7 +7244,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="334" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>12</v>
       </c>
@@ -7260,7 +7264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="335" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>12</v>
       </c>
@@ -7280,7 +7284,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="336" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>12</v>
       </c>
@@ -7300,7 +7304,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="337" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>12</v>
       </c>
@@ -7320,7 +7324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="338" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>12</v>
       </c>
@@ -7340,7 +7344,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="339" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>12</v>
       </c>
@@ -7360,7 +7364,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="340" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>12</v>
       </c>
@@ -7380,7 +7384,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="341" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>12</v>
       </c>
@@ -7400,7 +7404,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="342" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>12</v>
       </c>
@@ -7420,7 +7424,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="343" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>12</v>
       </c>
@@ -7440,7 +7444,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="344" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>12</v>
       </c>
@@ -7460,7 +7464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="345" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>12</v>
       </c>
@@ -7480,7 +7484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="346" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>12</v>
       </c>
@@ -7500,7 +7504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="347" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>12</v>
       </c>
@@ -7520,7 +7524,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="348" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>12</v>
       </c>
@@ -7540,7 +7544,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="349" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>12</v>
       </c>
@@ -7560,7 +7564,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="350" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>12</v>
       </c>
@@ -7580,7 +7584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="351" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>12</v>
       </c>
@@ -7600,7 +7604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="352" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>12</v>
       </c>
@@ -7620,7 +7624,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="353" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>12</v>
       </c>
@@ -7640,7 +7644,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="354" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>12</v>
       </c>
@@ -7660,7 +7664,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="355" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>12</v>
       </c>
@@ -7680,7 +7684,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="356" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>12</v>
       </c>
@@ -7700,7 +7704,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="357" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>12</v>
       </c>
@@ -7720,7 +7724,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="358" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>12</v>
       </c>
@@ -7740,7 +7744,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="359" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>12</v>
       </c>
@@ -7760,7 +7764,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="360" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>12</v>
       </c>
@@ -7780,7 +7784,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="361" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>12</v>
       </c>
@@ -7800,7 +7804,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="362" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>12</v>
       </c>
@@ -7820,7 +7824,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="363" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>12</v>
       </c>
@@ -7840,7 +7844,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="364" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>12</v>
       </c>
@@ -7860,7 +7864,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="365" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>12</v>
       </c>
@@ -7880,7 +7884,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="366" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>12</v>
       </c>
@@ -7900,7 +7904,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="367" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>12</v>
       </c>
@@ -7920,7 +7924,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="368" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>12</v>
       </c>
@@ -7940,7 +7944,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="369" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>12</v>
       </c>
@@ -7960,7 +7964,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="370" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>12</v>
       </c>
@@ -7980,7 +7984,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="371" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>12</v>
       </c>
@@ -8000,7 +8004,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="372" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>12</v>
       </c>
@@ -8020,7 +8024,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="373" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>12</v>
       </c>
@@ -8040,7 +8044,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="374" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>12</v>
       </c>
@@ -8060,7 +8064,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="375" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>12</v>
       </c>
@@ -8080,7 +8084,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="376" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>12</v>
       </c>
@@ -8100,7 +8104,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="377" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>12</v>
       </c>
@@ -8120,7 +8124,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="378" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>12</v>
       </c>
@@ -8140,7 +8144,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="379" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>12</v>
       </c>
@@ -8160,7 +8164,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="380" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>12</v>
       </c>
@@ -8180,7 +8184,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="381" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>12</v>
       </c>
@@ -8200,7 +8204,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="382" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>12</v>
       </c>
@@ -8220,7 +8224,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="383" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>12</v>
       </c>
@@ -8240,7 +8244,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="384" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>12</v>
       </c>
@@ -8260,7 +8264,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="385" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>12</v>
       </c>
@@ -8280,7 +8284,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="386" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>12</v>
       </c>
@@ -8300,7 +8304,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="387" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>12</v>
       </c>
@@ -8320,7 +8324,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="388" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>12</v>
       </c>
@@ -8340,7 +8344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="389" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>12</v>
       </c>
@@ -8360,7 +8364,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="390" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>12</v>
       </c>
@@ -8380,7 +8384,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="391" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>12</v>
       </c>
@@ -8400,7 +8404,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="392" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>12</v>
       </c>
@@ -8420,7 +8424,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="393" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>12</v>
       </c>
@@ -8440,7 +8444,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="394" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>12</v>
       </c>
@@ -8460,7 +8464,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="395" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>12</v>
       </c>
@@ -8480,7 +8484,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="396" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>12</v>
       </c>
@@ -8500,7 +8504,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="397" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>12</v>
       </c>
@@ -8520,7 +8524,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="398" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>12</v>
       </c>
@@ -8540,7 +8544,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="399" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>12</v>
       </c>
@@ -8560,7 +8564,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="400" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>12</v>
       </c>
@@ -8580,7 +8584,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="401" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>12</v>
       </c>
@@ -8600,7 +8604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="402" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>12</v>
       </c>
@@ -8620,7 +8624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="403" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>12</v>
       </c>
@@ -8640,7 +8644,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="404" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>12</v>
       </c>
@@ -8660,7 +8664,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="405" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>12</v>
       </c>
@@ -8680,7 +8684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="406" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>12</v>
       </c>
@@ -8700,7 +8704,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="407" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>12</v>
       </c>
@@ -8720,7 +8724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="408" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>12</v>
       </c>
@@ -16146,7 +16150,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="791" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="791" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A791" t="s">
         <v>20</v>
       </c>
@@ -16163,7 +16167,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="792" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="792" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A792" t="s">
         <v>20</v>
       </c>
@@ -16180,7 +16184,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="793" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="793" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A793" t="s">
         <v>20</v>
       </c>
@@ -16197,7 +16201,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="794" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="794" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A794" t="s">
         <v>20</v>
       </c>
@@ -16214,7 +16218,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="795" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="795" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A795" t="s">
         <v>20</v>
       </c>
@@ -16234,7 +16238,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="796" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="796" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A796" t="s">
         <v>20</v>
       </c>
@@ -16254,7 +16258,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="797" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="797" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A797" t="s">
         <v>20</v>
       </c>
@@ -16274,7 +16278,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="798" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="798" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A798" t="s">
         <v>20</v>
       </c>
@@ -16294,7 +16298,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="799" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="799" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A799" t="s">
         <v>20</v>
       </c>
@@ -16314,7 +16318,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="800" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="800" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A800" t="s">
         <v>20</v>
       </c>
@@ -16334,7 +16338,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="801" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="801" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A801" t="s">
         <v>20</v>
       </c>
@@ -16354,7 +16358,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="802" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="802" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A802" t="s">
         <v>20</v>
       </c>
@@ -16374,7 +16378,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="803" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="803" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A803" t="s">
         <v>20</v>
       </c>
@@ -16394,7 +16398,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="804" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="804" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A804" t="s">
         <v>20</v>
       </c>
@@ -16414,7 +16418,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="805" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="805" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A805" t="s">
         <v>20</v>
       </c>
@@ -16434,7 +16438,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="806" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="806" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A806" t="s">
         <v>20</v>
       </c>
@@ -16451,7 +16455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="807" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="807" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A807" t="s">
         <v>20</v>
       </c>
@@ -16468,7 +16472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="808" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="808" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A808" t="s">
         <v>20</v>
       </c>
@@ -16485,7 +16489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="809" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="809" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A809" t="s">
         <v>20</v>
       </c>
@@ -16502,7 +16506,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="810" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="810" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A810" t="s">
         <v>20</v>
       </c>
@@ -16519,7 +16523,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="811" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="811" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A811" t="s">
         <v>20</v>
       </c>
@@ -16536,7 +16540,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="812" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="812" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A812" t="s">
         <v>20</v>
       </c>
@@ -16553,7 +16557,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="813" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="813" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A813" t="s">
         <v>20</v>
       </c>
@@ -16573,7 +16577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="814" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="814" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A814" t="s">
         <v>20</v>
       </c>
@@ -16593,7 +16597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="815" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="815" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A815" t="s">
         <v>20</v>
       </c>
@@ -16613,7 +16617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="816" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="816" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A816" t="s">
         <v>20</v>
       </c>
@@ -16633,7 +16637,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="817" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="817" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A817" t="s">
         <v>20</v>
       </c>
@@ -16653,7 +16657,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="818" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="818" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A818" t="s">
         <v>20</v>
       </c>
@@ -16673,7 +16677,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="819" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="819" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A819" t="s">
         <v>20</v>
       </c>
@@ -16693,7 +16697,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="820" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="820" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A820" t="s">
         <v>20</v>
       </c>
@@ -16713,7 +16717,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="821" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="821" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A821" t="s">
         <v>20</v>
       </c>
@@ -16733,7 +16737,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="822" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="822" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A822" t="s">
         <v>20</v>
       </c>
@@ -16753,7 +16757,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="823" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="823" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A823" t="s">
         <v>20</v>
       </c>
@@ -16773,7 +16777,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="824" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="824" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A824" t="s">
         <v>20</v>
       </c>
@@ -16793,7 +16797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="825" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="825" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A825" t="s">
         <v>20</v>
       </c>
@@ -16813,7 +16817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="826" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="826" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A826" t="s">
         <v>20</v>
       </c>
@@ -16833,7 +16837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="827" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="827" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A827" t="s">
         <v>20</v>
       </c>
@@ -16853,7 +16857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="828" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="828" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A828" t="s">
         <v>20</v>
       </c>
@@ -16873,7 +16877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="829" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="829" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A829" t="s">
         <v>20</v>
       </c>
@@ -16893,7 +16897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="830" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="830" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A830" t="s">
         <v>20</v>
       </c>
@@ -16913,7 +16917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="831" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="831" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A831" t="s">
         <v>20</v>
       </c>
@@ -16933,7 +16937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="832" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="832" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A832" t="s">
         <v>20</v>
       </c>
@@ -16953,7 +16957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="833" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="833" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A833" t="s">
         <v>20</v>
       </c>
@@ -16973,7 +16977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="834" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="834" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A834" t="s">
         <v>20</v>
       </c>
@@ -16993,7 +16997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="835" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="835" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A835" t="s">
         <v>20</v>
       </c>
@@ -17013,7 +17017,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="836" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="836" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A836" t="s">
         <v>20</v>
       </c>
@@ -17033,7 +17037,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="837" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="837" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A837" t="s">
         <v>20</v>
       </c>
@@ -17053,7 +17057,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="838" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="838" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A838" t="s">
         <v>20</v>
       </c>
@@ -17073,7 +17077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="839" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="839" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A839" t="s">
         <v>20</v>
       </c>
@@ -17093,7 +17097,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="840" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="840" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A840" t="s">
         <v>20</v>
       </c>
@@ -17110,7 +17114,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="841" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="841" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A841" t="s">
         <v>20</v>
       </c>
@@ -17127,7 +17131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="842" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="842" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A842" t="s">
         <v>20</v>
       </c>
@@ -24300,7 +24304,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="1214" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1214" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1214" t="s">
         <v>28</v>
       </c>
@@ -24314,7 +24318,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="1215" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1215" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1215" t="s">
         <v>28</v>
       </c>
@@ -24331,7 +24335,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="1216" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1216" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1216" t="s">
         <v>28</v>
       </c>
@@ -24348,7 +24352,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="1217" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1217" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1217" t="s">
         <v>28</v>
       </c>
@@ -24365,7 +24369,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="1218" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1218" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1218" t="s">
         <v>28</v>
       </c>
@@ -24382,7 +24386,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="1219" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1219" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1219" t="s">
         <v>28</v>
       </c>
@@ -24399,7 +24403,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="1220" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1220" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1220" t="s">
         <v>28</v>
       </c>
@@ -24419,7 +24423,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1221" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1221" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1221" t="s">
         <v>28</v>
       </c>
@@ -24439,7 +24443,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1222" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1222" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1222" t="s">
         <v>28</v>
       </c>
@@ -24459,7 +24463,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1223" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1223" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1223" t="s">
         <v>28</v>
       </c>
@@ -24479,7 +24483,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="1224" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1224" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1224" t="s">
         <v>28</v>
       </c>
@@ -24499,7 +24503,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="1225" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1225" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1225" t="s">
         <v>28</v>
       </c>
@@ -24519,7 +24523,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="1226" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1226" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1226" t="s">
         <v>28</v>
       </c>
@@ -24539,7 +24543,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="1227" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1227" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1227" t="s">
         <v>28</v>
       </c>
@@ -24559,7 +24563,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1228" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1228" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1228" t="s">
         <v>28</v>
       </c>
@@ -24579,7 +24583,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="1229" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1229" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1229" t="s">
         <v>28</v>
       </c>
@@ -24599,7 +24603,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1230" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1230" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1230" t="s">
         <v>28</v>
       </c>
@@ -24619,7 +24623,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1231" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1231" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1231" t="s">
         <v>28</v>
       </c>
@@ -24639,7 +24643,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1232" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1232" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1232" t="s">
         <v>28</v>
       </c>
@@ -24659,7 +24663,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1233" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1233" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1233" t="s">
         <v>28</v>
       </c>
@@ -24679,7 +24683,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1234" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1234" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1234" t="s">
         <v>28</v>
       </c>
@@ -24699,7 +24703,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1235" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1235" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1235" t="s">
         <v>28</v>
       </c>
@@ -24719,7 +24723,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1236" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1236" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1236" t="s">
         <v>28</v>
       </c>
@@ -24739,7 +24743,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1237" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1237" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1237" t="s">
         <v>28</v>
       </c>
@@ -24759,7 +24763,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="1238" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1238" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1238" t="s">
         <v>28</v>
       </c>
@@ -24779,7 +24783,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="1239" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1239" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1239" t="s">
         <v>28</v>
       </c>
@@ -24799,7 +24803,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="1240" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1240" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1240" t="s">
         <v>28</v>
       </c>
@@ -24819,7 +24823,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="1241" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1241" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1241" t="s">
         <v>28</v>
       </c>
@@ -24839,7 +24843,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="1242" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1242" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1242" t="s">
         <v>28</v>
       </c>
@@ -24859,7 +24863,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="1243" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1243" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1243" t="s">
         <v>28</v>
       </c>
@@ -24879,7 +24883,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="1244" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1244" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1244" t="s">
         <v>28</v>
       </c>
@@ -24899,7 +24903,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="1245" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1245" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1245" t="s">
         <v>28</v>
       </c>
@@ -24919,7 +24923,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="1246" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1246" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1246" t="s">
         <v>28</v>
       </c>
@@ -24939,7 +24943,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1247" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1247" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1247" t="s">
         <v>28</v>
       </c>
@@ -24959,7 +24963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="1248" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1248" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1248" t="s">
         <v>28</v>
       </c>
@@ -24979,7 +24983,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="1249" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1249" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1249" t="s">
         <v>28</v>
       </c>
@@ -24999,7 +25003,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1250" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1250" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1250" t="s">
         <v>28</v>
       </c>
@@ -25019,7 +25023,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="1251" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1251" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1251" t="s">
         <v>28</v>
       </c>
@@ -25039,7 +25043,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="1252" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1252" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1252" t="s">
         <v>28</v>
       </c>
@@ -25059,7 +25063,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="1253" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1253" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1253" t="s">
         <v>28</v>
       </c>
@@ -25079,7 +25083,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="1254" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1254" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1254" t="s">
         <v>28</v>
       </c>
@@ -25099,7 +25103,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="1255" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1255" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1255" t="s">
         <v>28</v>
       </c>
@@ -25119,7 +25123,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1256" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1256" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1256" t="s">
         <v>28</v>
       </c>
@@ -25139,7 +25143,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="1257" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1257" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1257" t="s">
         <v>28</v>
       </c>
@@ -25159,7 +25163,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="1258" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1258" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1258" t="s">
         <v>28</v>
       </c>
@@ -25179,7 +25183,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="1259" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1259" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1259" t="s">
         <v>28</v>
       </c>
@@ -25199,7 +25203,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="1260" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1260" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1260" t="s">
         <v>28</v>
       </c>
@@ -25219,7 +25223,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="1261" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1261" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1261" t="s">
         <v>28</v>
       </c>
@@ -25239,7 +25243,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="1262" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1262" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1262" t="s">
         <v>28</v>
       </c>
@@ -25259,7 +25263,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1263" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1263" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1263" t="s">
         <v>28</v>
       </c>
@@ -25279,7 +25283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1264" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1264" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1264" t="s">
         <v>28</v>
       </c>
@@ -25299,7 +25303,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="1265" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1265" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1265" t="s">
         <v>28</v>
       </c>
@@ -25319,7 +25323,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="1266" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1266" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1266" t="s">
         <v>28</v>
       </c>
@@ -25339,7 +25343,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="1267" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1267" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1267" t="s">
         <v>28</v>
       </c>
@@ -25359,7 +25363,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="1268" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1268" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1268" t="s">
         <v>28</v>
       </c>
@@ -25379,7 +25383,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="1269" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1269" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1269" t="s">
         <v>28</v>
       </c>
@@ -25399,7 +25403,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="1270" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1270" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1270" t="s">
         <v>28</v>
       </c>
@@ -25419,7 +25423,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1271" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1271" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1271" t="s">
         <v>28</v>
       </c>
@@ -25439,7 +25443,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="1272" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1272" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1272" t="s">
         <v>28</v>
       </c>
@@ -25459,7 +25463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1273" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1273" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1273" t="s">
         <v>28</v>
       </c>
@@ -25479,7 +25483,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="1274" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1274" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1274" t="s">
         <v>28</v>
       </c>
@@ -25499,7 +25503,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="1275" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1275" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1275" t="s">
         <v>28</v>
       </c>
@@ -25519,7 +25523,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="1276" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1276" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1276" t="s">
         <v>28</v>
       </c>
@@ -25539,7 +25543,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="1277" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1277" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1277" t="s">
         <v>28</v>
       </c>
@@ -25559,7 +25563,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="1278" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1278" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1278" t="s">
         <v>28</v>
       </c>
@@ -25579,7 +25583,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="1279" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1279" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1279" t="s">
         <v>28</v>
       </c>
@@ -25599,7 +25603,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="1280" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1280" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1280" t="s">
         <v>28</v>
       </c>
@@ -25619,7 +25623,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="1281" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1281" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1281" t="s">
         <v>28</v>
       </c>
@@ -25639,7 +25643,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1282" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1282" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1282" t="s">
         <v>28</v>
       </c>
@@ -25659,7 +25663,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1283" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1283" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1283" t="s">
         <v>28</v>
       </c>
@@ -25679,7 +25683,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1284" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1284" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1284" t="s">
         <v>28</v>
       </c>
@@ -25699,7 +25703,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1285" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1285" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1285" t="s">
         <v>28</v>
       </c>
@@ -25719,7 +25723,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="1286" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1286" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1286" t="s">
         <v>28</v>
       </c>
@@ -25739,7 +25743,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1287" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1287" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1287" t="s">
         <v>28</v>
       </c>
@@ -25759,7 +25763,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="1288" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1288" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1288" t="s">
         <v>28</v>
       </c>
@@ -25779,7 +25783,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="1289" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1289" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1289" t="s">
         <v>28</v>
       </c>
@@ -25799,7 +25803,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="1290" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1290" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1290" t="s">
         <v>28</v>
       </c>
@@ -25819,7 +25823,7 @@
         <v>-21</v>
       </c>
     </row>
-    <row r="1291" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1291" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1291" t="s">
         <v>28</v>
       </c>
@@ -25839,7 +25843,7 @@
         <v>-25</v>
       </c>
     </row>
-    <row r="1292" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1292" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1292" t="s">
         <v>28</v>
       </c>
@@ -25859,7 +25863,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="1293" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1293" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1293" t="s">
         <v>28</v>
       </c>
@@ -25879,7 +25883,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="1294" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1294" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1294" t="s">
         <v>28</v>
       </c>
@@ -25899,7 +25903,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="1295" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1295" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1295" t="s">
         <v>28</v>
       </c>
@@ -25919,7 +25923,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="1296" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1296" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1296" t="s">
         <v>28</v>
       </c>
@@ -25939,7 +25943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1297" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1297" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1297" t="s">
         <v>28</v>
       </c>
@@ -25959,7 +25963,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="1298" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1298" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1298" t="s">
         <v>28</v>
       </c>
@@ -25979,7 +25983,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1299" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1299" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1299" t="s">
         <v>28</v>
       </c>
@@ -25999,7 +26003,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1300" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1300" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1300" t="s">
         <v>28</v>
       </c>
@@ -26019,7 +26023,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1301" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1301" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1301" t="s">
         <v>28</v>
       </c>
@@ -26039,7 +26043,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1302" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1302" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1302" t="s">
         <v>28</v>
       </c>
@@ -26059,7 +26063,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1303" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1303" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1303" t="s">
         <v>28</v>
       </c>
@@ -26079,7 +26083,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1304" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1304" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1304" t="s">
         <v>28</v>
       </c>
@@ -26099,7 +26103,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="1305" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1305" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1305" t="s">
         <v>28</v>
       </c>
@@ -26119,7 +26123,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="1306" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1306" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1306" t="s">
         <v>28</v>
       </c>
@@ -26139,7 +26143,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="1307" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1307" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1307" t="s">
         <v>29</v>
       </c>
@@ -26156,7 +26160,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="1308" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1308" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1308" t="s">
         <v>29</v>
       </c>
@@ -26173,7 +26177,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="1309" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1309" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1309" t="s">
         <v>29</v>
       </c>
@@ -26190,7 +26194,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="1310" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1310" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1310" t="s">
         <v>29</v>
       </c>
@@ -26207,7 +26211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="1311" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1311" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1311" t="s">
         <v>29</v>
       </c>
@@ -26227,7 +26231,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="1312" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1312" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1312" t="s">
         <v>29</v>
       </c>
@@ -26247,7 +26251,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="1313" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1313" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1313" t="s">
         <v>29</v>
       </c>
@@ -26267,7 +26271,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="1314" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1314" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1314" t="s">
         <v>29</v>
       </c>
@@ -26287,7 +26291,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1315" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1315" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1315" t="s">
         <v>29</v>
       </c>
@@ -26307,7 +26311,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1316" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1316" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1316" t="s">
         <v>29</v>
       </c>
@@ -26327,7 +26331,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1317" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1317" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1317" t="s">
         <v>29</v>
       </c>
@@ -26347,7 +26351,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="1318" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1318" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1318" t="s">
         <v>29</v>
       </c>
@@ -26367,7 +26371,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="1319" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1319" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1319" t="s">
         <v>29</v>
       </c>
@@ -26387,7 +26391,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1320" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1320" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1320" t="s">
         <v>29</v>
       </c>
@@ -26407,7 +26411,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="1321" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1321" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1321" t="s">
         <v>29</v>
       </c>
@@ -26427,7 +26431,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="1322" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1322" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1322" t="s">
         <v>29</v>
       </c>
@@ -27621,11 +27625,7 @@
   <autoFilter ref="A1:F1382" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="ABNB"/>
-        <filter val="BKNG"/>
-        <filter val="Orbitz"/>
-        <filter val="Webjet"/>
-        <filter val="Webjet OTA"/>
+        <filter val="EXPE"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>